<commit_message>
Refactoring of Framework of Lesson 4 FOR MySQL part 1
</commit_message>
<xml_diff>
--- a/AndyTEST/Libs/ComplexScenariosChecklist.xlsx
+++ b/AndyTEST/Libs/ComplexScenariosChecklist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="-45" windowWidth="14835" windowHeight="13980" tabRatio="595"/>
@@ -1824,917 +1824,917 @@
     <t>175.</t>
   </si>
   <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1001</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1002</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1003</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1004</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1005</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1006</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1007</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1008</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1009</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1010</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1011</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1012</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1013</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1014</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1015</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1016</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1017</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1018</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1019</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1020</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1021</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1022</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1023</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1024</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1025</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1026</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1027</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1028</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1029</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1030</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1031</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1032</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1033</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1034</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1035</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1001</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1002</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1003</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1004</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1005</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1006</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1007</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1008</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1009</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1010</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1011</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1012</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1013</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1014</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1015</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1016</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1017</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1018</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1019</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1020</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1021</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1022</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1023</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1024</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1025</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1026</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1027</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1028</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1029</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1030</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1031</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1032</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1033</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1034</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1035</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t>SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1002</t>
+  </si>
+  <si>
+    <t>SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1003</t>
+  </si>
+  <si>
+    <t>SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1004</t>
+  </si>
+  <si>
+    <t>SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1005</t>
+  </si>
+  <si>
+    <t>SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1006</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1007</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1008</t>
+  </si>
+  <si>
+    <t>SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1009</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1010</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1011</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1012</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1013</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1014</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1015</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1017</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1018</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1019</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1020</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1022</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1023</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1024</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1025</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1026</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1027</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1028</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1029</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1030</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1031</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1032</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1033</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1034</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT dutyFree, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1035</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1002</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1003</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1004</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1005</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1006</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1007</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1008</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1009</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1010</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1011</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1012</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1013</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1014</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1015</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1017</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1018</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1019</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1020</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1022</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1023</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1024</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1025</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1026</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1027</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1028</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1029</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1030</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1031</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1032</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1033</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1034</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT priorityBoarding, departureAirport FROM Airports INNER JOIN Flights ON Airports.airportNumber=Flights.airportNumber WHERE flightNumber = 1035</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1001</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1002</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1003</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1004</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1005</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1006</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1007</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1008</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1009</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1010</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1011</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1012</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1013</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1014</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1015</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1016</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1017</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1018</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1019</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1020</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1021</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1022</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1023</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1024</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1025</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1026</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1027</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1028</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1029</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1030</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1031</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1032</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1033</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1034</t>
   </si>
   <si>
-    <t>USE TestDB SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT departureAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1035</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1001</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1002</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1003</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1004</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1005</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1006</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1007</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1008</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1009</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1010</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1011</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1012</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1013</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1014</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1015</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1016</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1017</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1018</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1019</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1020</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1021</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1022</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1023</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1024</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1025</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1026</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1027</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1028</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1029</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1030</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1031</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1032</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1033</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1034</t>
   </si>
   <si>
-    <t>USE TestDB SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT arrivalAirport, airline FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1035</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1001</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1002</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1003</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1004</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1005</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1006</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1007</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1008</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1009</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1010</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1011</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1012</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1013</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1014</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1015</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1016</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1017</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1018</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1019</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1020</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1021</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1022</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1023</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1024</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1025</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1026</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1027</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1028</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1029</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1030</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1031</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1032</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1033</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1034</t>
   </si>
   <si>
-    <t>USE TestDB SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT stopsNumber, additionalSpaceService FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1035</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1001</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1002</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1003</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1004</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1005</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1006</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1007</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1008</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1009</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1010</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1011</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1012</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1013</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1014</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1015</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1016</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1017</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1018</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1019</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1020</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1021</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1022</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1023</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1024</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1025</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1026</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1027</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1028</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1029</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1030</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1031</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1032</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1033</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1034</t>
   </si>
   <si>
-    <t>USE TestDB SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT averageTicketPrice, webRegistration FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1035</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1001</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1002</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1003</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1004</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1005</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1006</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1007</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1008</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1009</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1010</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1011</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1012</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1013</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1014</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1015</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1016</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1017</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1018</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1019</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1020</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1021</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1022</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1023</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1024</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1025</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1026</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1027</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1028</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1029</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1030</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1031</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1032</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1033</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1034</t>
   </si>
   <si>
-    <t>USE TestDB SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
+    <t xml:space="preserve"> SELECT availableSeats, isMealIncluded FROM Flights INNER JOIN Airlines 
 ON Flights.flightNumber =Airlines.flightNumber  WHERE Flights.flightNumber = 1035</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2742,7 +2742,7 @@
 WHERE Airlines.flightNumber = 1001</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2750,7 +2750,7 @@
 WHERE Airlines.flightNumber = 1002</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2758,7 +2758,7 @@
 WHERE Airlines.flightNumber = 1003</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2766,7 +2766,7 @@
 WHERE Airlines.flightNumber = 1004</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2774,7 +2774,15 @@
 WHERE Airlines.flightNumber = 1005</t>
   </si>
   <si>
-    <t>USE TestDBSELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
+INNER JOIN Flights 
+ON Airports.airportNumber = Flights.airportNumber
+INNER JOIN  Airlines
+ON Flights.flightNumber = Airlines.flightNumber
+WHERE Airlines.flightNumber = 1006</t>
+  </si>
+  <si>
+    <t>SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2782,15 +2790,7 @@
 WHERE Airlines.flightNumber = 1007</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
-INNER JOIN Flights 
-ON Airports.airportNumber = Flights.airportNumber
-INNER JOIN  Airlines
-ON Flights.flightNumber = Airlines.flightNumber
-WHERE Airlines.flightNumber = 1006</t>
-  </si>
-  <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2798,7 +2798,7 @@
 WHERE Airlines.flightNumber = 1008</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2806,7 +2806,7 @@
 WHERE Airlines.flightNumber = 1009</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2814,7 +2814,7 @@
 WHERE Airlines.flightNumber = 1010</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2822,7 +2822,7 @@
 WHERE Airlines.flightNumber = 1011</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2830,7 +2830,7 @@
 WHERE Airlines.flightNumber = 1012</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2838,7 +2838,7 @@
 WHERE Airlines.flightNumber = 1013</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2846,7 +2846,7 @@
 WHERE Airlines.flightNumber = 1014</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2854,7 +2854,7 @@
 WHERE Airlines.flightNumber = 1015</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2862,7 +2862,7 @@
 WHERE Airlines.flightNumber = 1016</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2870,7 +2870,7 @@
 WHERE Airlines.flightNumber = 1017</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2878,7 +2878,7 @@
 WHERE Airlines.flightNumber = 1018</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2886,7 +2886,7 @@
 WHERE Airlines.flightNumber = 1019</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2894,7 +2894,7 @@
 WHERE Airlines.flightNumber = 1020</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2902,7 +2902,7 @@
 WHERE Airlines.flightNumber = 1021</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2910,7 +2910,7 @@
 WHERE Airlines.flightNumber = 1022</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2918,7 +2918,7 @@
 WHERE Airlines.flightNumber = 1023</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2926,7 +2926,7 @@
 WHERE Airlines.flightNumber = 1024</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2934,7 +2934,7 @@
 WHERE Airlines.flightNumber = 1025</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2942,7 +2942,7 @@
 WHERE Airlines.flightNumber = 1026</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2950,7 +2950,7 @@
 WHERE Airlines.flightNumber = 1027</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2958,7 +2958,7 @@
 WHERE Airlines.flightNumber = 1028</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2966,7 +2966,7 @@
 WHERE Airlines.flightNumber = 1029</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2974,7 +2974,7 @@
 WHERE Airlines.flightNumber = 1030</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2982,7 +2982,7 @@
 WHERE Airlines.flightNumber = 1031</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2990,7 +2990,7 @@
 WHERE Airlines.flightNumber = 1032</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -2998,7 +2998,7 @@
 WHERE Airlines.flightNumber = 1033</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -3006,7 +3006,7 @@
 WHERE Airlines.flightNumber = 1034</t>
   </si>
   <si>
-    <t>USE TestDB SELECT priorityBoarding, webRegistration FROM Airports 
+    <t xml:space="preserve"> SELECT priorityBoarding, webRegistration FROM Airports 
 INNER JOIN Flights 
 ON Airports.airportNumber = Flights.airportNumber
 INNER JOIN  Airlines
@@ -6309,13 +6309,13 @@
     <xf numFmtId="0" fontId="246" fillId="247" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6378,7 +6378,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6413,7 +6413,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6625,17 +6625,17 @@
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="55.75" style="11" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="44.875" style="11" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.125" style="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.75" style="11" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.75" style="11" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="55.7109375" style="11" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="44.85546875" style="11" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.140625" style="11" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.7109375" style="11" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.7109375" style="11" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -7218,7 +7218,7 @@
       <c r="E36" s="9"/>
       <c r="F36" s="46"/>
     </row>
-    <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>462</v>
       </c>
@@ -7234,7 +7234,7 @@
       <c r="E37" s="10"/>
       <c r="F37" s="47"/>
     </row>
-    <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>463</v>
       </c>
@@ -7250,7 +7250,7 @@
       <c r="E38" s="10"/>
       <c r="F38" s="48"/>
     </row>
-    <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>464</v>
       </c>
@@ -7266,7 +7266,7 @@
       <c r="E39" s="10"/>
       <c r="F39" s="49"/>
     </row>
-    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>465</v>
       </c>
@@ -7282,7 +7282,7 @@
       <c r="E40" s="10"/>
       <c r="F40" s="50"/>
     </row>
-    <row r="41" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>466</v>
       </c>
@@ -7298,7 +7298,7 @@
       <c r="E41" s="10"/>
       <c r="F41" s="51"/>
     </row>
-    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>467</v>
       </c>
@@ -7314,7 +7314,7 @@
       <c r="E42" s="10"/>
       <c r="F42" s="52"/>
     </row>
-    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>468</v>
       </c>
@@ -7330,7 +7330,7 @@
       <c r="E43" s="10"/>
       <c r="F43" s="53"/>
     </row>
-    <row r="44" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>469</v>
       </c>
@@ -7346,7 +7346,7 @@
       <c r="E44" s="10"/>
       <c r="F44" s="54"/>
     </row>
-    <row r="45" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>470</v>
       </c>
@@ -7362,7 +7362,7 @@
       <c r="E45" s="10"/>
       <c r="F45" s="55"/>
     </row>
-    <row r="46" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>471</v>
       </c>
@@ -7378,7 +7378,7 @@
       <c r="E46" s="10"/>
       <c r="F46" s="56"/>
     </row>
-    <row r="47" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>472</v>
       </c>
@@ -7394,7 +7394,7 @@
       <c r="E47" s="10"/>
       <c r="F47" s="57"/>
     </row>
-    <row r="48" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>473</v>
       </c>
@@ -7410,7 +7410,7 @@
       <c r="E48" s="10"/>
       <c r="F48" s="58"/>
     </row>
-    <row r="49" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>474</v>
       </c>
@@ -7426,7 +7426,7 @@
       <c r="E49" s="10"/>
       <c r="F49" s="59"/>
     </row>
-    <row r="50" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>475</v>
       </c>
@@ -7442,7 +7442,7 @@
       <c r="E50" s="10"/>
       <c r="F50" s="60"/>
     </row>
-    <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>476</v>
       </c>
@@ -7458,7 +7458,7 @@
       <c r="E51" s="10"/>
       <c r="F51" s="61"/>
     </row>
-    <row r="52" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>477</v>
       </c>
@@ -7474,7 +7474,7 @@
       <c r="E52" s="10"/>
       <c r="F52" s="62"/>
     </row>
-    <row r="53" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>478</v>
       </c>
@@ -7490,7 +7490,7 @@
       <c r="E53" s="10"/>
       <c r="F53" s="63"/>
     </row>
-    <row r="54" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>479</v>
       </c>
@@ -7506,7 +7506,7 @@
       <c r="E54" s="10"/>
       <c r="F54" s="64"/>
     </row>
-    <row r="55" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>480</v>
       </c>
@@ -7522,7 +7522,7 @@
       <c r="E55" s="10"/>
       <c r="F55" s="65"/>
     </row>
-    <row r="56" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>481</v>
       </c>
@@ -7538,7 +7538,7 @@
       <c r="E56" s="10"/>
       <c r="F56" s="66"/>
     </row>
-    <row r="57" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>482</v>
       </c>
@@ -7554,7 +7554,7 @@
       <c r="E57" s="10"/>
       <c r="F57" s="67"/>
     </row>
-    <row r="58" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>483</v>
       </c>
@@ -7570,7 +7570,7 @@
       <c r="E58" s="10"/>
       <c r="F58" s="68"/>
     </row>
-    <row r="59" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>484</v>
       </c>
@@ -7586,7 +7586,7 @@
       <c r="E59" s="10"/>
       <c r="F59" s="69"/>
     </row>
-    <row r="60" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>485</v>
       </c>
@@ -7602,7 +7602,7 @@
       <c r="E60" s="10"/>
       <c r="F60" s="70"/>
     </row>
-    <row r="61" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>486</v>
       </c>
@@ -7618,7 +7618,7 @@
       <c r="E61" s="10"/>
       <c r="F61" s="71"/>
     </row>
-    <row r="62" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>487</v>
       </c>
@@ -7634,7 +7634,7 @@
       <c r="E62" s="10"/>
       <c r="F62" s="72"/>
     </row>
-    <row r="63" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>488</v>
       </c>
@@ -7650,7 +7650,7 @@
       <c r="E63" s="10"/>
       <c r="F63" s="73"/>
     </row>
-    <row r="64" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>489</v>
       </c>
@@ -7666,7 +7666,7 @@
       <c r="E64" s="10"/>
       <c r="F64" s="74"/>
     </row>
-    <row r="65" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>490</v>
       </c>
@@ -7682,7 +7682,7 @@
       <c r="E65" s="10"/>
       <c r="F65" s="75"/>
     </row>
-    <row r="66" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>491</v>
       </c>
@@ -7698,7 +7698,7 @@
       <c r="E66" s="10"/>
       <c r="F66" s="76"/>
     </row>
-    <row r="67" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>492</v>
       </c>
@@ -7714,7 +7714,7 @@
       <c r="E67" s="10"/>
       <c r="F67" s="77"/>
     </row>
-    <row r="68" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>493</v>
       </c>
@@ -7730,7 +7730,7 @@
       <c r="E68" s="10"/>
       <c r="F68" s="78"/>
     </row>
-    <row r="69" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>494</v>
       </c>
@@ -7746,7 +7746,7 @@
       <c r="E69" s="10"/>
       <c r="F69" s="79"/>
     </row>
-    <row r="70" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>495</v>
       </c>
@@ -7762,7 +7762,7 @@
       <c r="E70" s="10"/>
       <c r="F70" s="80"/>
     </row>
-    <row r="71" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>496</v>
       </c>
@@ -7795,10 +7795,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="51.875" style="11" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="41.875" style="11" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.875" style="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.125" style="11" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="51.85546875" style="11" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="41.85546875" style="11" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.85546875" style="11" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.140625" style="11" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="14" style="11" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -7822,7 +7822,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>427</v>
       </c>
@@ -7838,7 +7838,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="83"/>
     </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>428</v>
       </c>
@@ -7854,7 +7854,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="84"/>
     </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>429</v>
       </c>
@@ -7870,7 +7870,7 @@
       <c r="E4" s="9"/>
       <c r="F4" s="85"/>
     </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>430</v>
       </c>
@@ -7886,7 +7886,7 @@
       <c r="E5" s="9"/>
       <c r="F5" s="86"/>
     </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>431</v>
       </c>
@@ -7902,7 +7902,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="87"/>
     </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>432</v>
       </c>
@@ -7918,7 +7918,7 @@
       <c r="E7" s="9"/>
       <c r="F7" s="88"/>
     </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>433</v>
       </c>
@@ -7934,7 +7934,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="89"/>
     </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>434</v>
       </c>
@@ -7950,7 +7950,7 @@
       <c r="E9" s="9"/>
       <c r="F9" s="90"/>
     </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>435</v>
       </c>
@@ -7966,7 +7966,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="91"/>
     </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>436</v>
       </c>
@@ -7982,7 +7982,7 @@
       <c r="E11" s="9"/>
       <c r="F11" s="92"/>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>437</v>
       </c>
@@ -7998,7 +7998,7 @@
       <c r="E12" s="9"/>
       <c r="F12" s="93"/>
     </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>438</v>
       </c>
@@ -8014,7 +8014,7 @@
       <c r="E13" s="9"/>
       <c r="F13" s="94"/>
     </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>439</v>
       </c>
@@ -8030,7 +8030,7 @@
       <c r="E14" s="9"/>
       <c r="F14" s="95"/>
     </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>440</v>
       </c>
@@ -8046,7 +8046,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="96"/>
     </row>
-    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>441</v>
       </c>
@@ -8062,7 +8062,7 @@
       <c r="E16" s="9"/>
       <c r="F16" s="97"/>
     </row>
-    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>442</v>
       </c>
@@ -8078,7 +8078,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="98"/>
     </row>
-    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>443</v>
       </c>
@@ -8094,7 +8094,7 @@
       <c r="E18" s="9"/>
       <c r="F18" s="99"/>
     </row>
-    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>444</v>
       </c>
@@ -8110,7 +8110,7 @@
       <c r="E19" s="9"/>
       <c r="F19" s="100"/>
     </row>
-    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>445</v>
       </c>
@@ -8126,7 +8126,7 @@
       <c r="E20" s="9"/>
       <c r="F20" s="101"/>
     </row>
-    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>446</v>
       </c>
@@ -8142,7 +8142,7 @@
       <c r="E21" s="9"/>
       <c r="F21" s="102"/>
     </row>
-    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>447</v>
       </c>
@@ -8158,7 +8158,7 @@
       <c r="E22" s="9"/>
       <c r="F22" s="103"/>
     </row>
-    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>448</v>
       </c>
@@ -8174,7 +8174,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="104"/>
     </row>
-    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>449</v>
       </c>
@@ -8190,7 +8190,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="105"/>
     </row>
-    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>450</v>
       </c>
@@ -8206,7 +8206,7 @@
       <c r="E25" s="9"/>
       <c r="F25" s="106"/>
     </row>
-    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>451</v>
       </c>
@@ -8222,7 +8222,7 @@
       <c r="E26" s="9"/>
       <c r="F26" s="107"/>
     </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>452</v>
       </c>
@@ -8238,7 +8238,7 @@
       <c r="E27" s="9"/>
       <c r="F27" s="108"/>
     </row>
-    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>453</v>
       </c>
@@ -8254,7 +8254,7 @@
       <c r="E28" s="9"/>
       <c r="F28" s="109"/>
     </row>
-    <row r="29" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>454</v>
       </c>
@@ -8270,7 +8270,7 @@
       <c r="E29" s="9"/>
       <c r="F29" s="110"/>
     </row>
-    <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>455</v>
       </c>
@@ -8286,7 +8286,7 @@
       <c r="E30" s="9"/>
       <c r="F30" s="111"/>
     </row>
-    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>456</v>
       </c>
@@ -8302,7 +8302,7 @@
       <c r="E31" s="9"/>
       <c r="F31" s="112"/>
     </row>
-    <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>457</v>
       </c>
@@ -8318,7 +8318,7 @@
       <c r="E32" s="9"/>
       <c r="F32" s="113"/>
     </row>
-    <row r="33" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>458</v>
       </c>
@@ -8334,7 +8334,7 @@
       <c r="E33" s="9"/>
       <c r="F33" s="114"/>
     </row>
-    <row r="34" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>459</v>
       </c>
@@ -8350,7 +8350,7 @@
       <c r="E34" s="9"/>
       <c r="F34" s="115"/>
     </row>
-    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>460</v>
       </c>
@@ -8366,7 +8366,7 @@
       <c r="E35" s="9"/>
       <c r="F35" s="116"/>
     </row>
-    <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>461</v>
       </c>
@@ -8382,7 +8382,7 @@
       <c r="E36" s="9"/>
       <c r="F36" s="117"/>
     </row>
-    <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>462</v>
       </c>
@@ -8398,7 +8398,7 @@
       <c r="E37" s="10"/>
       <c r="F37" s="118"/>
     </row>
-    <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>463</v>
       </c>
@@ -8414,7 +8414,7 @@
       <c r="E38" s="10"/>
       <c r="F38" s="119"/>
     </row>
-    <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>464</v>
       </c>
@@ -8430,7 +8430,7 @@
       <c r="E39" s="10"/>
       <c r="F39" s="120"/>
     </row>
-    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>465</v>
       </c>
@@ -8446,7 +8446,7 @@
       <c r="E40" s="10"/>
       <c r="F40" s="121"/>
     </row>
-    <row r="41" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>466</v>
       </c>
@@ -8462,7 +8462,7 @@
       <c r="E41" s="10"/>
       <c r="F41" s="122"/>
     </row>
-    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>467</v>
       </c>
@@ -8478,7 +8478,7 @@
       <c r="E42" s="10"/>
       <c r="F42" s="123"/>
     </row>
-    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>468</v>
       </c>
@@ -8494,7 +8494,7 @@
       <c r="E43" s="10"/>
       <c r="F43" s="124"/>
     </row>
-    <row r="44" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>469</v>
       </c>
@@ -8510,7 +8510,7 @@
       <c r="E44" s="10"/>
       <c r="F44" s="125"/>
     </row>
-    <row r="45" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>470</v>
       </c>
@@ -8526,7 +8526,7 @@
       <c r="E45" s="10"/>
       <c r="F45" s="126"/>
     </row>
-    <row r="46" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>471</v>
       </c>
@@ -8542,7 +8542,7 @@
       <c r="E46" s="10"/>
       <c r="F46" s="127"/>
     </row>
-    <row r="47" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>472</v>
       </c>
@@ -8558,7 +8558,7 @@
       <c r="E47" s="10"/>
       <c r="F47" s="128"/>
     </row>
-    <row r="48" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>473</v>
       </c>
@@ -8574,7 +8574,7 @@
       <c r="E48" s="10"/>
       <c r="F48" s="129"/>
     </row>
-    <row r="49" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>474</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="E49" s="10"/>
       <c r="F49" s="130"/>
     </row>
-    <row r="50" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>475</v>
       </c>
@@ -8606,7 +8606,7 @@
       <c r="E50" s="10"/>
       <c r="F50" s="131"/>
     </row>
-    <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>476</v>
       </c>
@@ -8622,7 +8622,7 @@
       <c r="E51" s="10"/>
       <c r="F51" s="132"/>
     </row>
-    <row r="52" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>477</v>
       </c>
@@ -8638,7 +8638,7 @@
       <c r="E52" s="10"/>
       <c r="F52" s="133"/>
     </row>
-    <row r="53" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>478</v>
       </c>
@@ -8654,7 +8654,7 @@
       <c r="E53" s="10"/>
       <c r="F53" s="134"/>
     </row>
-    <row r="54" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>479</v>
       </c>
@@ -8670,7 +8670,7 @@
       <c r="E54" s="10"/>
       <c r="F54" s="135"/>
     </row>
-    <row r="55" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>480</v>
       </c>
@@ -8686,7 +8686,7 @@
       <c r="E55" s="10"/>
       <c r="F55" s="136"/>
     </row>
-    <row r="56" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>481</v>
       </c>
@@ -8702,7 +8702,7 @@
       <c r="E56" s="10"/>
       <c r="F56" s="137"/>
     </row>
-    <row r="57" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>482</v>
       </c>
@@ -8718,7 +8718,7 @@
       <c r="E57" s="10"/>
       <c r="F57" s="138"/>
     </row>
-    <row r="58" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>483</v>
       </c>
@@ -8734,7 +8734,7 @@
       <c r="E58" s="10"/>
       <c r="F58" s="139"/>
     </row>
-    <row r="59" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>484</v>
       </c>
@@ -8750,7 +8750,7 @@
       <c r="E59" s="10"/>
       <c r="F59" s="140"/>
     </row>
-    <row r="60" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>485</v>
       </c>
@@ -8766,7 +8766,7 @@
       <c r="E60" s="10"/>
       <c r="F60" s="141"/>
     </row>
-    <row r="61" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>486</v>
       </c>
@@ -8782,7 +8782,7 @@
       <c r="E61" s="10"/>
       <c r="F61" s="142"/>
     </row>
-    <row r="62" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>487</v>
       </c>
@@ -8798,7 +8798,7 @@
       <c r="E62" s="10"/>
       <c r="F62" s="143"/>
     </row>
-    <row r="63" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>488</v>
       </c>
@@ -8814,7 +8814,7 @@
       <c r="E63" s="10"/>
       <c r="F63" s="144"/>
     </row>
-    <row r="64" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>489</v>
       </c>
@@ -8830,7 +8830,7 @@
       <c r="E64" s="10"/>
       <c r="F64" s="145"/>
     </row>
-    <row r="65" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>490</v>
       </c>
@@ -8846,7 +8846,7 @@
       <c r="E65" s="10"/>
       <c r="F65" s="146"/>
     </row>
-    <row r="66" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>491</v>
       </c>
@@ -8862,7 +8862,7 @@
       <c r="E66" s="10"/>
       <c r="F66" s="147"/>
     </row>
-    <row r="67" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>492</v>
       </c>
@@ -8878,7 +8878,7 @@
       <c r="E67" s="10"/>
       <c r="F67" s="148"/>
     </row>
-    <row r="68" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>493</v>
       </c>
@@ -8894,7 +8894,7 @@
       <c r="E68" s="10"/>
       <c r="F68" s="149"/>
     </row>
-    <row r="69" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>494</v>
       </c>
@@ -8910,7 +8910,7 @@
       <c r="E69" s="10"/>
       <c r="F69" s="150"/>
     </row>
-    <row r="70" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>495</v>
       </c>
@@ -8926,7 +8926,7 @@
       <c r="E70" s="10"/>
       <c r="F70" s="151"/>
     </row>
-    <row r="71" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>496</v>
       </c>
@@ -8942,7 +8942,7 @@
       <c r="E71" s="10"/>
       <c r="F71" s="152"/>
     </row>
-    <row r="72" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>497</v>
       </c>
@@ -8958,7 +8958,7 @@
       <c r="E72" s="9"/>
       <c r="F72" s="153"/>
     </row>
-    <row r="73" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>498</v>
       </c>
@@ -8974,7 +8974,7 @@
       <c r="E73" s="9"/>
       <c r="F73" s="154"/>
     </row>
-    <row r="74" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>499</v>
       </c>
@@ -8990,7 +8990,7 @@
       <c r="E74" s="9"/>
       <c r="F74" s="155"/>
     </row>
-    <row r="75" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>500</v>
       </c>
@@ -9006,7 +9006,7 @@
       <c r="E75" s="9"/>
       <c r="F75" s="156"/>
     </row>
-    <row r="76" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>501</v>
       </c>
@@ -9022,7 +9022,7 @@
       <c r="E76" s="9"/>
       <c r="F76" s="157"/>
     </row>
-    <row r="77" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>502</v>
       </c>
@@ -9038,7 +9038,7 @@
       <c r="E77" s="9"/>
       <c r="F77" s="158"/>
     </row>
-    <row r="78" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>503</v>
       </c>
@@ -9054,7 +9054,7 @@
       <c r="E78" s="9"/>
       <c r="F78" s="159"/>
     </row>
-    <row r="79" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>504</v>
       </c>
@@ -9070,7 +9070,7 @@
       <c r="E79" s="9"/>
       <c r="F79" s="160"/>
     </row>
-    <row r="80" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>505</v>
       </c>
@@ -9086,7 +9086,7 @@
       <c r="E80" s="9"/>
       <c r="F80" s="161"/>
     </row>
-    <row r="81" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>506</v>
       </c>
@@ -9102,7 +9102,7 @@
       <c r="E81" s="9"/>
       <c r="F81" s="162"/>
     </row>
-    <row r="82" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>507</v>
       </c>
@@ -9118,7 +9118,7 @@
       <c r="E82" s="9"/>
       <c r="F82" s="163"/>
     </row>
-    <row r="83" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>508</v>
       </c>
@@ -9134,7 +9134,7 @@
       <c r="E83" s="9"/>
       <c r="F83" s="164"/>
     </row>
-    <row r="84" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>509</v>
       </c>
@@ -9150,7 +9150,7 @@
       <c r="E84" s="9"/>
       <c r="F84" s="165"/>
     </row>
-    <row r="85" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>510</v>
       </c>
@@ -9166,7 +9166,7 @@
       <c r="E85" s="9"/>
       <c r="F85" s="166"/>
     </row>
-    <row r="86" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>511</v>
       </c>
@@ -9182,7 +9182,7 @@
       <c r="E86" s="9"/>
       <c r="F86" s="167"/>
     </row>
-    <row r="87" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>512</v>
       </c>
@@ -9198,7 +9198,7 @@
       <c r="E87" s="9"/>
       <c r="F87" s="168"/>
     </row>
-    <row r="88" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>513</v>
       </c>
@@ -9214,7 +9214,7 @@
       <c r="E88" s="9"/>
       <c r="F88" s="169"/>
     </row>
-    <row r="89" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>514</v>
       </c>
@@ -9230,7 +9230,7 @@
       <c r="E89" s="9"/>
       <c r="F89" s="170"/>
     </row>
-    <row r="90" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>515</v>
       </c>
@@ -9246,7 +9246,7 @@
       <c r="E90" s="9"/>
       <c r="F90" s="171"/>
     </row>
-    <row r="91" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>516</v>
       </c>
@@ -9262,7 +9262,7 @@
       <c r="E91" s="9"/>
       <c r="F91" s="172"/>
     </row>
-    <row r="92" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>517</v>
       </c>
@@ -9278,7 +9278,7 @@
       <c r="E92" s="9"/>
       <c r="F92" s="173"/>
     </row>
-    <row r="93" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>518</v>
       </c>
@@ -9294,7 +9294,7 @@
       <c r="E93" s="9"/>
       <c r="F93" s="174"/>
     </row>
-    <row r="94" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>519</v>
       </c>
@@ -9310,7 +9310,7 @@
       <c r="E94" s="9"/>
       <c r="F94" s="175"/>
     </row>
-    <row r="95" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>520</v>
       </c>
@@ -9326,7 +9326,7 @@
       <c r="E95" s="9"/>
       <c r="F95" s="176"/>
     </row>
-    <row r="96" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>521</v>
       </c>
@@ -9342,7 +9342,7 @@
       <c r="E96" s="9"/>
       <c r="F96" s="177"/>
     </row>
-    <row r="97" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>522</v>
       </c>
@@ -9358,7 +9358,7 @@
       <c r="E97" s="9"/>
       <c r="F97" s="178"/>
     </row>
-    <row r="98" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>523</v>
       </c>
@@ -9374,7 +9374,7 @@
       <c r="E98" s="9"/>
       <c r="F98" s="179"/>
     </row>
-    <row r="99" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>524</v>
       </c>
@@ -9390,7 +9390,7 @@
       <c r="E99" s="9"/>
       <c r="F99" s="180"/>
     </row>
-    <row r="100" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>525</v>
       </c>
@@ -9406,7 +9406,7 @@
       <c r="E100" s="9"/>
       <c r="F100" s="181"/>
     </row>
-    <row r="101" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>526</v>
       </c>
@@ -9422,7 +9422,7 @@
       <c r="E101" s="9"/>
       <c r="F101" s="182"/>
     </row>
-    <row r="102" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>527</v>
       </c>
@@ -9438,7 +9438,7 @@
       <c r="E102" s="9"/>
       <c r="F102" s="183"/>
     </row>
-    <row r="103" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>528</v>
       </c>
@@ -9454,7 +9454,7 @@
       <c r="E103" s="9"/>
       <c r="F103" s="184"/>
     </row>
-    <row r="104" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>529</v>
       </c>
@@ -9470,7 +9470,7 @@
       <c r="E104" s="9"/>
       <c r="F104" s="185"/>
     </row>
-    <row r="105" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>530</v>
       </c>
@@ -9486,7 +9486,7 @@
       <c r="E105" s="9"/>
       <c r="F105" s="186"/>
     </row>
-    <row r="106" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>531</v>
       </c>
@@ -9502,7 +9502,7 @@
       <c r="E106" s="9"/>
       <c r="F106" s="187"/>
     </row>
-    <row r="107" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>532</v>
       </c>
@@ -9518,7 +9518,7 @@
       <c r="E107" s="10"/>
       <c r="F107" s="188"/>
     </row>
-    <row r="108" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>533</v>
       </c>
@@ -9534,7 +9534,7 @@
       <c r="E108" s="10"/>
       <c r="F108" s="189"/>
     </row>
-    <row r="109" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>534</v>
       </c>
@@ -9550,7 +9550,7 @@
       <c r="E109" s="10"/>
       <c r="F109" s="190"/>
     </row>
-    <row r="110" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>535</v>
       </c>
@@ -9566,7 +9566,7 @@
       <c r="E110" s="10"/>
       <c r="F110" s="191"/>
     </row>
-    <row r="111" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>536</v>
       </c>
@@ -9582,7 +9582,7 @@
       <c r="E111" s="10"/>
       <c r="F111" s="192"/>
     </row>
-    <row r="112" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>537</v>
       </c>
@@ -9598,7 +9598,7 @@
       <c r="E112" s="10"/>
       <c r="F112" s="193"/>
     </row>
-    <row r="113" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>538</v>
       </c>
@@ -9614,7 +9614,7 @@
       <c r="E113" s="10"/>
       <c r="F113" s="194"/>
     </row>
-    <row r="114" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>539</v>
       </c>
@@ -9630,7 +9630,7 @@
       <c r="E114" s="10"/>
       <c r="F114" s="195"/>
     </row>
-    <row r="115" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>540</v>
       </c>
@@ -9646,7 +9646,7 @@
       <c r="E115" s="10"/>
       <c r="F115" s="196"/>
     </row>
-    <row r="116" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>541</v>
       </c>
@@ -9662,7 +9662,7 @@
       <c r="E116" s="10"/>
       <c r="F116" s="197"/>
     </row>
-    <row r="117" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>542</v>
       </c>
@@ -9678,7 +9678,7 @@
       <c r="E117" s="10"/>
       <c r="F117" s="198"/>
     </row>
-    <row r="118" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>543</v>
       </c>
@@ -9694,7 +9694,7 @@
       <c r="E118" s="10"/>
       <c r="F118" s="199"/>
     </row>
-    <row r="119" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>544</v>
       </c>
@@ -9710,7 +9710,7 @@
       <c r="E119" s="10"/>
       <c r="F119" s="200"/>
     </row>
-    <row r="120" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>545</v>
       </c>
@@ -9726,7 +9726,7 @@
       <c r="E120" s="10"/>
       <c r="F120" s="201"/>
     </row>
-    <row r="121" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>546</v>
       </c>
@@ -9742,7 +9742,7 @@
       <c r="E121" s="10"/>
       <c r="F121" s="202"/>
     </row>
-    <row r="122" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>547</v>
       </c>
@@ -9758,7 +9758,7 @@
       <c r="E122" s="10"/>
       <c r="F122" s="203"/>
     </row>
-    <row r="123" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>548</v>
       </c>
@@ -9774,7 +9774,7 @@
       <c r="E123" s="10"/>
       <c r="F123" s="204"/>
     </row>
-    <row r="124" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>549</v>
       </c>
@@ -9790,7 +9790,7 @@
       <c r="E124" s="10"/>
       <c r="F124" s="205"/>
     </row>
-    <row r="125" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>550</v>
       </c>
@@ -9806,7 +9806,7 @@
       <c r="E125" s="10"/>
       <c r="F125" s="206"/>
     </row>
-    <row r="126" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>551</v>
       </c>
@@ -9822,7 +9822,7 @@
       <c r="E126" s="10"/>
       <c r="F126" s="207"/>
     </row>
-    <row r="127" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>552</v>
       </c>
@@ -9838,7 +9838,7 @@
       <c r="E127" s="10"/>
       <c r="F127" s="208"/>
     </row>
-    <row r="128" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>553</v>
       </c>
@@ -9854,7 +9854,7 @@
       <c r="E128" s="10"/>
       <c r="F128" s="209"/>
     </row>
-    <row r="129" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>554</v>
       </c>
@@ -9870,7 +9870,7 @@
       <c r="E129" s="10"/>
       <c r="F129" s="210"/>
     </row>
-    <row r="130" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>555</v>
       </c>
@@ -9886,7 +9886,7 @@
       <c r="E130" s="10"/>
       <c r="F130" s="211"/>
     </row>
-    <row r="131" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>556</v>
       </c>
@@ -9902,7 +9902,7 @@
       <c r="E131" s="10"/>
       <c r="F131" s="212"/>
     </row>
-    <row r="132" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>557</v>
       </c>
@@ -9918,7 +9918,7 @@
       <c r="E132" s="10"/>
       <c r="F132" s="213"/>
     </row>
-    <row r="133" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>558</v>
       </c>
@@ -9934,7 +9934,7 @@
       <c r="E133" s="10"/>
       <c r="F133" s="214"/>
     </row>
-    <row r="134" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>559</v>
       </c>
@@ -9950,7 +9950,7 @@
       <c r="E134" s="10"/>
       <c r="F134" s="215"/>
     </row>
-    <row r="135" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>560</v>
       </c>
@@ -9966,7 +9966,7 @@
       <c r="E135" s="10"/>
       <c r="F135" s="216"/>
     </row>
-    <row r="136" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>561</v>
       </c>
@@ -9982,7 +9982,7 @@
       <c r="E136" s="10"/>
       <c r="F136" s="217"/>
     </row>
-    <row r="137" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>562</v>
       </c>
@@ -9998,7 +9998,7 @@
       <c r="E137" s="10"/>
       <c r="F137" s="218"/>
     </row>
-    <row r="138" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>563</v>
       </c>
@@ -10014,7 +10014,7 @@
       <c r="E138" s="10"/>
       <c r="F138" s="219"/>
     </row>
-    <row r="139" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>564</v>
       </c>
@@ -10030,7 +10030,7 @@
       <c r="E139" s="10"/>
       <c r="F139" s="220"/>
     </row>
-    <row r="140" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>565</v>
       </c>
@@ -10046,7 +10046,7 @@
       <c r="E140" s="10"/>
       <c r="F140" s="221"/>
     </row>
-    <row r="141" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>566</v>
       </c>
@@ -10062,7 +10062,7 @@
       <c r="E141" s="10"/>
       <c r="F141" s="222"/>
     </row>
-    <row r="142" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>567</v>
       </c>
@@ -10078,7 +10078,7 @@
       <c r="E142" s="9"/>
       <c r="F142" s="223"/>
     </row>
-    <row r="143" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>568</v>
       </c>
@@ -10094,7 +10094,7 @@
       <c r="E143" s="9"/>
       <c r="F143" s="224"/>
     </row>
-    <row r="144" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>569</v>
       </c>
@@ -10110,7 +10110,7 @@
       <c r="E144" s="9"/>
       <c r="F144" s="225"/>
     </row>
-    <row r="145" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>570</v>
       </c>
@@ -10126,7 +10126,7 @@
       <c r="E145" s="9"/>
       <c r="F145" s="226"/>
     </row>
-    <row r="146" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>571</v>
       </c>
@@ -10142,7 +10142,7 @@
       <c r="E146" s="9"/>
       <c r="F146" s="227"/>
     </row>
-    <row r="147" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>572</v>
       </c>
@@ -10158,7 +10158,7 @@
       <c r="E147" s="9"/>
       <c r="F147" s="228"/>
     </row>
-    <row r="148" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>573</v>
       </c>
@@ -10174,7 +10174,7 @@
       <c r="E148" s="9"/>
       <c r="F148" s="229"/>
     </row>
-    <row r="149" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>574</v>
       </c>
@@ -10190,7 +10190,7 @@
       <c r="E149" s="9"/>
       <c r="F149" s="230"/>
     </row>
-    <row r="150" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>575</v>
       </c>
@@ -10206,7 +10206,7 @@
       <c r="E150" s="9"/>
       <c r="F150" s="231"/>
     </row>
-    <row r="151" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>576</v>
       </c>
@@ -10222,7 +10222,7 @@
       <c r="E151" s="9"/>
       <c r="F151" s="232"/>
     </row>
-    <row r="152" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>577</v>
       </c>
@@ -10238,7 +10238,7 @@
       <c r="E152" s="9"/>
       <c r="F152" s="233"/>
     </row>
-    <row r="153" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>578</v>
       </c>
@@ -10254,7 +10254,7 @@
       <c r="E153" s="9"/>
       <c r="F153" s="234"/>
     </row>
-    <row r="154" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>579</v>
       </c>
@@ -10270,7 +10270,7 @@
       <c r="E154" s="9"/>
       <c r="F154" s="235"/>
     </row>
-    <row r="155" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>580</v>
       </c>
@@ -10286,7 +10286,7 @@
       <c r="E155" s="9"/>
       <c r="F155" s="236"/>
     </row>
-    <row r="156" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>581</v>
       </c>
@@ -10302,7 +10302,7 @@
       <c r="E156" s="9"/>
       <c r="F156" s="237"/>
     </row>
-    <row r="157" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>582</v>
       </c>
@@ -10318,7 +10318,7 @@
       <c r="E157" s="9"/>
       <c r="F157" s="238"/>
     </row>
-    <row r="158" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>583</v>
       </c>
@@ -10334,7 +10334,7 @@
       <c r="E158" s="9"/>
       <c r="F158" s="239"/>
     </row>
-    <row r="159" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>584</v>
       </c>
@@ -10350,7 +10350,7 @@
       <c r="E159" s="9"/>
       <c r="F159" s="240"/>
     </row>
-    <row r="160" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>585</v>
       </c>
@@ -10366,7 +10366,7 @@
       <c r="E160" s="9"/>
       <c r="F160" s="241"/>
     </row>
-    <row r="161" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>586</v>
       </c>
@@ -10382,7 +10382,7 @@
       <c r="E161" s="9"/>
       <c r="F161" s="242"/>
     </row>
-    <row r="162" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>587</v>
       </c>
@@ -10398,7 +10398,7 @@
       <c r="E162" s="9"/>
       <c r="F162" s="243"/>
     </row>
-    <row r="163" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>588</v>
       </c>
@@ -10414,7 +10414,7 @@
       <c r="E163" s="9"/>
       <c r="F163" s="244"/>
     </row>
-    <row r="164" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>589</v>
       </c>
@@ -10430,7 +10430,7 @@
       <c r="E164" s="9"/>
       <c r="F164" s="245"/>
     </row>
-    <row r="165" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>590</v>
       </c>
@@ -10446,7 +10446,7 @@
       <c r="E165" s="9"/>
       <c r="F165" s="246"/>
     </row>
-    <row r="166" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>591</v>
       </c>
@@ -10462,7 +10462,7 @@
       <c r="E166" s="9"/>
       <c r="F166" s="247"/>
     </row>
-    <row r="167" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>592</v>
       </c>
@@ -10478,7 +10478,7 @@
       <c r="E167" s="9"/>
       <c r="F167" s="248"/>
     </row>
-    <row r="168" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>593</v>
       </c>
@@ -10494,7 +10494,7 @@
       <c r="E168" s="9"/>
       <c r="F168" s="249"/>
     </row>
-    <row r="169" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>594</v>
       </c>
@@ -10510,7 +10510,7 @@
       <c r="E169" s="9"/>
       <c r="F169" s="250"/>
     </row>
-    <row r="170" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>595</v>
       </c>
@@ -10526,7 +10526,7 @@
       <c r="E170" s="9"/>
       <c r="F170" s="251"/>
     </row>
-    <row r="171" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>596</v>
       </c>
@@ -10542,7 +10542,7 @@
       <c r="E171" s="9"/>
       <c r="F171" s="252"/>
     </row>
-    <row r="172" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>597</v>
       </c>
@@ -10558,7 +10558,7 @@
       <c r="E172" s="9"/>
       <c r="F172" s="253"/>
     </row>
-    <row r="173" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>598</v>
       </c>
@@ -10574,7 +10574,7 @@
       <c r="E173" s="9"/>
       <c r="F173" s="254"/>
     </row>
-    <row r="174" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>599</v>
       </c>
@@ -10590,7 +10590,7 @@
       <c r="E174" s="9"/>
       <c r="F174" s="255"/>
     </row>
-    <row r="175" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>600</v>
       </c>
@@ -10606,7 +10606,7 @@
       <c r="E175" s="9"/>
       <c r="F175" s="256"/>
     </row>
-    <row r="176" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>601</v>
       </c>
@@ -10638,11 +10638,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.125" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="50.375" style="11" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.375" style="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.125" style="11" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.875" style="258" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="50.42578125" style="11" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" style="11" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.140625" style="11" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" style="260" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -10661,7 +10661,7 @@
       <c r="E1" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="F1" s="259" t="s">
+      <c r="F1" s="258" t="s">
         <v>285</v>
       </c>
     </row>
@@ -10679,7 +10679,7 @@
         <v>423</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="260"/>
+      <c r="F2" s="259"/>
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10696,7 +10696,7 @@
         <v>423</v>
       </c>
       <c r="E3" s="10"/>
-      <c r="F3" s="260"/>
+      <c r="F3" s="259"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10713,7 +10713,7 @@
         <v>424</v>
       </c>
       <c r="E4" s="10"/>
-      <c r="F4" s="260"/>
+      <c r="F4" s="259"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10730,7 +10730,7 @@
         <v>424</v>
       </c>
       <c r="E5" s="10"/>
-      <c r="F5" s="260"/>
+      <c r="F5" s="259"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10747,7 +10747,7 @@
         <v>425</v>
       </c>
       <c r="E6" s="10"/>
-      <c r="F6" s="260"/>
+      <c r="F6" s="259"/>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10758,13 +10758,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>425</v>
       </c>
       <c r="E7" s="10"/>
-      <c r="F7" s="260"/>
+      <c r="F7" s="259"/>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10775,13 +10775,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>425</v>
       </c>
       <c r="E8" s="10"/>
-      <c r="F8" s="260"/>
+      <c r="F8" s="259"/>
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10798,7 +10798,7 @@
         <v>425</v>
       </c>
       <c r="E9" s="10"/>
-      <c r="F9" s="260"/>
+      <c r="F9" s="259"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10815,7 +10815,7 @@
         <v>425</v>
       </c>
       <c r="E10" s="10"/>
-      <c r="F10" s="260"/>
+      <c r="F10" s="259"/>
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10832,7 +10832,7 @@
         <v>426</v>
       </c>
       <c r="E11" s="10"/>
-      <c r="F11" s="260"/>
+      <c r="F11" s="259"/>
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10849,7 +10849,7 @@
         <v>426</v>
       </c>
       <c r="E12" s="10"/>
-      <c r="F12" s="260"/>
+      <c r="F12" s="259"/>
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10866,7 +10866,7 @@
         <v>426</v>
       </c>
       <c r="E13" s="10"/>
-      <c r="F13" s="260"/>
+      <c r="F13" s="259"/>
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10883,7 +10883,7 @@
         <v>426</v>
       </c>
       <c r="E14" s="10"/>
-      <c r="F14" s="260"/>
+      <c r="F14" s="259"/>
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10900,7 +10900,7 @@
         <v>424</v>
       </c>
       <c r="E15" s="10"/>
-      <c r="F15" s="260"/>
+      <c r="F15" s="259"/>
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10917,7 +10917,7 @@
         <v>423</v>
       </c>
       <c r="E16" s="10"/>
-      <c r="F16" s="260"/>
+      <c r="F16" s="259"/>
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10934,7 +10934,7 @@
         <v>426</v>
       </c>
       <c r="E17" s="10"/>
-      <c r="F17" s="260"/>
+      <c r="F17" s="259"/>
       <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10951,7 +10951,7 @@
         <v>425</v>
       </c>
       <c r="E18" s="10"/>
-      <c r="F18" s="260"/>
+      <c r="F18" s="259"/>
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10968,7 +10968,7 @@
         <v>426</v>
       </c>
       <c r="E19" s="10"/>
-      <c r="F19" s="260"/>
+      <c r="F19" s="259"/>
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -10985,7 +10985,7 @@
         <v>423</v>
       </c>
       <c r="E20" s="10"/>
-      <c r="F20" s="260"/>
+      <c r="F20" s="259"/>
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -11002,7 +11002,7 @@
         <v>423</v>
       </c>
       <c r="E21" s="10"/>
-      <c r="F21" s="260"/>
+      <c r="F21" s="259"/>
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -11019,7 +11019,7 @@
         <v>423</v>
       </c>
       <c r="E22" s="10"/>
-      <c r="F22" s="260"/>
+      <c r="F22" s="259"/>
       <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -11036,7 +11036,7 @@
         <v>423</v>
       </c>
       <c r="E23" s="10"/>
-      <c r="F23" s="260"/>
+      <c r="F23" s="259"/>
       <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -11053,7 +11053,7 @@
         <v>424</v>
       </c>
       <c r="E24" s="10"/>
-      <c r="F24" s="260"/>
+      <c r="F24" s="259"/>
       <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -11070,7 +11070,7 @@
         <v>423</v>
       </c>
       <c r="E25" s="10"/>
-      <c r="F25" s="260"/>
+      <c r="F25" s="259"/>
       <c r="G25" s="6"/>
     </row>
     <row r="26" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -11087,7 +11087,7 @@
         <v>426</v>
       </c>
       <c r="E26" s="10"/>
-      <c r="F26" s="260"/>
+      <c r="F26" s="259"/>
       <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -11104,7 +11104,7 @@
         <v>425</v>
       </c>
       <c r="E27" s="10"/>
-      <c r="F27" s="260"/>
+      <c r="F27" s="259"/>
       <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -11121,7 +11121,7 @@
         <v>426</v>
       </c>
       <c r="E28" s="10"/>
-      <c r="F28" s="260"/>
+      <c r="F28" s="259"/>
       <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -11138,7 +11138,7 @@
         <v>425</v>
       </c>
       <c r="E29" s="10"/>
-      <c r="F29" s="260"/>
+      <c r="F29" s="259"/>
       <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -11155,7 +11155,7 @@
         <v>426</v>
       </c>
       <c r="E30" s="10"/>
-      <c r="F30" s="260"/>
+      <c r="F30" s="259"/>
       <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -11172,7 +11172,7 @@
         <v>423</v>
       </c>
       <c r="E31" s="10"/>
-      <c r="F31" s="260"/>
+      <c r="F31" s="259"/>
       <c r="G31" s="6"/>
     </row>
     <row r="32" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -11189,7 +11189,7 @@
         <v>425</v>
       </c>
       <c r="E32" s="10"/>
-      <c r="F32" s="260"/>
+      <c r="F32" s="259"/>
       <c r="G32" s="6"/>
     </row>
     <row r="33" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -11206,7 +11206,7 @@
         <v>426</v>
       </c>
       <c r="E33" s="10"/>
-      <c r="F33" s="260"/>
+      <c r="F33" s="259"/>
       <c r="G33" s="6"/>
     </row>
     <row r="34" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -11223,7 +11223,7 @@
         <v>424</v>
       </c>
       <c r="E34" s="10"/>
-      <c r="F34" s="260"/>
+      <c r="F34" s="259"/>
       <c r="G34" s="6"/>
     </row>
     <row r="35" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -11240,7 +11240,7 @@
         <v>424</v>
       </c>
       <c r="E35" s="10"/>
-      <c r="F35" s="260"/>
+      <c r="F35" s="259"/>
       <c r="G35" s="6"/>
     </row>
     <row r="36" spans="1:7" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -11257,7 +11257,7 @@
         <v>424</v>
       </c>
       <c r="E36" s="10"/>
-      <c r="F36" s="260"/>
+      <c r="F36" s="259"/>
       <c r="G36" s="6"/>
     </row>
   </sheetData>

</xml_diff>